<commit_message>
Task planning update 1.1
</commit_message>
<xml_diff>
--- a/TownHallTaskPlanning.xlsx
+++ b/TownHallTaskPlanning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miky\Documents\GitHub\InformationSystemsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Task planning update 1.2
</commit_message>
<xml_diff>
--- a/TownHallTaskPlanning.xlsx
+++ b/TownHallTaskPlanning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miky\Documents\GitHub\InformationSystemsProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miky\Documents\Visual Studio 2017\Projects\TownHall\TownHall\wwwroot\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>